<commit_message>
In the midst of regression testing.
</commit_message>
<xml_diff>
--- a/testing/iteration 5/REGRESSION Testing- Iter 5.xlsx
+++ b/testing/iteration 5/REGRESSION Testing- Iter 5.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Overuse" sheetId="12" r:id="rId6"/>
     <sheet name="Heatmap" sheetId="10" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="185">
   <si>
     <t>TEST CASES</t>
   </si>
@@ -629,12 +629,81 @@
   <si>
     <t>Need to update with time</t>
   </si>
+  <si>
+    <t>Regression Testing(Iteration5)</t>
+  </si>
+  <si>
+    <t>Returns -1 for all blocks</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Row 7 did not return a timestamp error</t>
+  </si>
+  <si>
+    <t>Only return 1 error message</t>
+  </si>
+  <si>
+    <t>It shows no error with records</t>
+  </si>
+  <si>
+    <t>Regression Testing (Iteration5)</t>
+  </si>
+  <si>
+    <t>Returned no matching mac address,invalid app instead of duplicates</t>
+  </si>
+  <si>
+    <t>Wrong error messages for different rows</t>
+  </si>
+  <si>
+    <t>Crashes with nullpointer exception</t>
+  </si>
+  <si>
+    <t>Regression Testing(Iteration 5)</t>
+  </si>
+  <si>
+    <t>Overuse results: Overusing
+Usage results: Severe
+23312
+Gaming Usage results: Moderate
+3944
+Access Frequency results: Light
+0.96</t>
+  </si>
+  <si>
+    <t>Overuse results: Overusing
+Usage results: Moderate
+13133
+Gaming Usage results: Severe
+10851
+Access Frequency results: Light
+0.66</t>
+  </si>
+  <si>
+    <t>Overuse results: Overusing
+Usage results: Severe
+18190
+Gaming Usage results: Severe
+15566
+Access Frequency results: Light
+1.25</t>
+  </si>
+  <si>
+    <t>Overuse results: Overusing
+Usage results: Severe
+31382
+Gaming Usage results: Severe
+19645
+Access Frequency results: Light
+1.38</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -727,6 +796,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -842,7 +918,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -939,6 +1015,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1402,10 +1481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="66" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="C5" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="66" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1417,9 +1496,10 @@
     <col min="6" max="6" width="35.83203125" customWidth="1"/>
     <col min="7" max="7" width="12.58203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -1433,8 +1513,11 @@
       <c r="I1" s="19" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1465,8 +1548,11 @@
       <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="K2" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1497,8 +1583,14 @@
       <c r="J3" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="K3" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1529,8 +1621,14 @@
       <c r="J4" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="93" x14ac:dyDescent="0.35">
+      <c r="K4" t="s">
+        <v>171</v>
+      </c>
+      <c r="L4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="93" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1561,8 +1659,14 @@
       <c r="J5" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="170.5" x14ac:dyDescent="0.35">
+      <c r="K5" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1593,8 +1697,14 @@
       <c r="J6" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="K6" t="s">
+        <v>173</v>
+      </c>
+      <c r="L6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1625,8 +1735,14 @@
       <c r="J7" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="K7" t="s">
+        <v>174</v>
+      </c>
+      <c r="L7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1657,8 +1773,14 @@
       <c r="J8" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8" t="s">
+        <v>175</v>
+      </c>
+      <c r="L8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1682,10 +1804,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J7"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1698,17 +1820,21 @@
     <col min="6" max="6" width="78.33203125" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="G1" t="s">
         <v>117</v>
       </c>
       <c r="I1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -1739,8 +1865,14 @@
       <c r="J2" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -1771,8 +1903,14 @@
       <c r="J3" s="13" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K3" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="L3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -1803,8 +1941,14 @@
       <c r="J4" s="13" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K4" t="s">
+        <v>178</v>
+      </c>
+      <c r="L4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -1835,8 +1979,14 @@
       <c r="J5" s="13" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K5" t="s">
+        <v>178</v>
+      </c>
+      <c r="L5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -1867,8 +2017,14 @@
       <c r="J6" s="13" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K6" t="s">
+        <v>178</v>
+      </c>
+      <c r="L6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -1898,6 +2054,12 @@
       </c>
       <c r="J7" s="13" t="s">
         <v>89</v>
+      </c>
+      <c r="K7" t="s">
+        <v>179</v>
+      </c>
+      <c r="L7" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1916,7 +2078,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2444,7 +2606,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2469,7 +2631,7 @@
       <c r="E1" s="32"/>
       <c r="F1" s="7"/>
       <c r="G1" s="1" t="s">
-        <v>118</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -2626,10 +2788,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2645,7 +2807,7 @@
     <col min="10" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
         <v>133</v>
       </c>
@@ -2660,7 +2822,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
@@ -2689,7 +2851,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="22">
         <v>1</v>
       </c>
@@ -2715,7 +2877,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="26" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" s="26" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="22">
         <v>2</v>
       </c>
@@ -2741,7 +2903,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="26" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" s="26" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22">
         <v>3</v>
       </c>
@@ -2768,7 +2930,7 @@
       </c>
       <c r="I5" s="27"/>
     </row>
-    <row r="6" spans="1:9" s="26" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" s="26" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="22">
         <v>4</v>
       </c>
@@ -2794,7 +2956,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="26" customFormat="1" ht="124" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" s="26" customFormat="1" ht="124" x14ac:dyDescent="0.35">
       <c r="A7" s="22">
         <v>5</v>
       </c>
@@ -2819,8 +2981,14 @@
       <c r="H7" s="22" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="26" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="I7" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="26" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A8" s="22">
         <v>6</v>
       </c>
@@ -2845,8 +3013,14 @@
       <c r="H8" s="22" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" s="26" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+      <c r="I8" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="26" customFormat="1" ht="93" x14ac:dyDescent="0.35">
       <c r="A9" s="22">
         <v>7</v>
       </c>
@@ -2871,8 +3045,11 @@
       <c r="H9" s="22" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="26" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+      <c r="I9" s="26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="26" customFormat="1" ht="93" x14ac:dyDescent="0.35">
       <c r="A10" s="22">
         <v>8</v>
       </c>
@@ -2896,6 +3073,9 @@
       </c>
       <c r="H10" s="22" t="s">
         <v>90</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>